<commit_message>
Dataset Distribution files updated
</commit_message>
<xml_diff>
--- a/KeyphraseListPreparation/Dataset Distribution.xlsx
+++ b/KeyphraseListPreparation/Dataset Distribution.xlsx
@@ -38,9 +38,6 @@
     <t>For keyphrase list preparation</t>
   </si>
   <si>
-    <t>For testing</t>
-  </si>
-  <si>
     <t>business</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>tech</t>
+  </si>
+  <si>
+    <t>For summarization evaluation</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +572,7 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.88671875" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -595,12 +595,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
         <v>510</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>386</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="6" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>414</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="7" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>511</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="8" spans="2:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="10">
         <v>401</v>

</xml_diff>